<commit_message>
completed assignment 3 and starting assignment 4
</commit_message>
<xml_diff>
--- a/Intro to Machine Learning/Assignment_2_Data_and_Template.xlsx
+++ b/Intro to Machine Learning/Assignment_2_Data_and_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="30">
   <si>
     <t>Sex</t>
   </si>
@@ -58,7 +58,7 @@
     <t>No. of bins</t>
   </si>
   <si>
-    <t>22x11</t>
+    <t>9x9</t>
   </si>
   <si>
     <t>No. of bins to be decided by student upto max 32x32</t>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>     17.5</t>
-  </si>
-  <si>
-    <t>Indeterminate</t>
   </si>
   <si>
     <t>     22</t>
@@ -2536,7 +2533,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2667,7 +2664,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>26</v>
+        <v>25.5</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -2726,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="18">
         <v>0</v>
@@ -2743,12 +2740,8 @@
       <c r="J7" s="18">
         <v>0</v>
       </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
@@ -2773,19 +2766,19 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="18">
         <v>0</v>
@@ -2799,12 +2792,8 @@
       <c r="J8" s="18">
         <v>0</v>
       </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
@@ -2829,22 +2818,22 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="18">
         <v>0</v>
       </c>
       <c r="D9" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="18">
         <v>0</v>
@@ -2855,12 +2844,8 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -2888,20 +2873,20 @@
         <v>0</v>
       </c>
       <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>13</v>
+      </c>
+      <c r="E10" s="18">
+        <v>11</v>
+      </c>
+      <c r="F10" s="18">
+        <v>7</v>
+      </c>
+      <c r="G10" s="18">
         <v>1</v>
       </c>
-      <c r="D10" s="18">
-        <v>1</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
       <c r="H10" s="18">
         <v>0</v>
       </c>
@@ -2911,12 +2896,8 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <v>0</v>
-      </c>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
@@ -2944,22 +2925,22 @@
         <v>0</v>
       </c>
       <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18">
         <v>2</v>
       </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
       <c r="E11" s="18">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F11" s="18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="18">
         <v>0</v>
@@ -2967,12 +2948,8 @@
       <c r="J11" s="18">
         <v>0</v>
       </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
@@ -3000,13 +2977,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="18">
+        <v>0</v>
+      </c>
+      <c r="D12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="E12" s="18">
         <v>1</v>
-      </c>
-      <c r="E12" s="18">
-        <v>0</v>
       </c>
       <c r="F12" s="18">
         <v>1</v>
@@ -3023,12 +3000,8 @@
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -3053,7 +3026,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="18">
         <v>0</v>
@@ -3062,13 +3035,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" s="18">
         <v>0</v>
@@ -3079,12 +3052,8 @@
       <c r="J13" s="18">
         <v>0</v>
       </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -3112,22 +3081,22 @@
         <v>0</v>
       </c>
       <c r="C14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="18">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E14" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="18">
         <v>0</v>
@@ -3135,12 +3104,8 @@
       <c r="J14" s="18">
         <v>0</v>
       </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
@@ -3174,13 +3139,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="18">
         <v>0</v>
@@ -3191,12 +3156,8 @@
       <c r="J15" s="18">
         <v>0</v>
       </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -3220,39 +3181,17 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>2</v>
-      </c>
-      <c r="E16" s="18">
-        <v>2</v>
-      </c>
-      <c r="F16" s="18">
-        <v>4</v>
-      </c>
-      <c r="G16" s="18">
-        <v>2</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0</v>
-      </c>
-      <c r="K16" s="18">
-        <v>0</v>
-      </c>
-      <c r="L16" s="18">
-        <v>0</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -3276,39 +3215,17 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0</v>
-      </c>
-      <c r="D17" s="18">
-        <v>1</v>
-      </c>
-      <c r="E17" s="18">
-        <v>4</v>
-      </c>
-      <c r="F17" s="18">
-        <v>8</v>
-      </c>
-      <c r="G17" s="18">
-        <v>1</v>
-      </c>
-      <c r="H17" s="18">
-        <v>0</v>
-      </c>
-      <c r="I17" s="18">
-        <v>0</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -3332,39 +3249,17 @@
       <c r="AG17" s="18"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>2</v>
-      </c>
-      <c r="F18" s="18">
-        <v>4</v>
-      </c>
-      <c r="G18" s="18">
-        <v>4</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0</v>
-      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -3388,39 +3283,17 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <v>1</v>
-      </c>
-      <c r="E19" s="18">
-        <v>1</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0</v>
-      </c>
-      <c r="I19" s="18">
-        <v>0</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0</v>
-      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -3444,39 +3317,17 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0</v>
-      </c>
-      <c r="I20" s="18">
-        <v>0</v>
-      </c>
-      <c r="J20" s="18">
-        <v>0</v>
-      </c>
-      <c r="K20" s="18">
-        <v>0</v>
-      </c>
-      <c r="L20" s="18">
-        <v>0</v>
-      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -3500,39 +3351,17 @@
       <c r="AG20" s="18"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0</v>
-      </c>
-      <c r="I21" s="18">
-        <v>0</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0</v>
-      </c>
-      <c r="K21" s="18">
-        <v>0</v>
-      </c>
-      <c r="L21" s="18">
-        <v>0</v>
-      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -3556,39 +3385,17 @@
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B22" s="18">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <v>0</v>
-      </c>
-      <c r="G22" s="18">
-        <v>1</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0</v>
-      </c>
-      <c r="I22" s="18">
-        <v>0</v>
-      </c>
-      <c r="J22" s="18">
-        <v>0</v>
-      </c>
-      <c r="K22" s="18">
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
-        <v>0</v>
-      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -3612,39 +3419,17 @@
       <c r="AG22" s="18"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0</v>
-      </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
-        <v>0</v>
-      </c>
-      <c r="J23" s="18">
-        <v>0</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
-        <v>0</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
@@ -3668,39 +3453,17 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B24" s="18">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <v>0</v>
-      </c>
-      <c r="I24" s="18">
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
-        <v>0</v>
-      </c>
-      <c r="K24" s="18">
-        <v>0</v>
-      </c>
-      <c r="L24" s="18">
-        <v>0</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
@@ -3724,39 +3487,17 @@
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <v>0</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <v>0</v>
-      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
@@ -3780,39 +3521,17 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B26" s="18">
-        <v>0</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0</v>
-      </c>
-      <c r="D26" s="18">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="18">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
-        <v>0</v>
-      </c>
-      <c r="K26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <v>0</v>
-      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -3836,39 +3555,17 @@
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B27" s="18">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0</v>
-      </c>
-      <c r="D27" s="18">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <v>0</v>
-      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -3892,39 +3589,17 @@
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <v>0</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18">
-        <v>0</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
-        <v>0</v>
-      </c>
-      <c r="L28" s="18">
-        <v>0</v>
-      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
@@ -4296,8 +3971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4428,7 +4103,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>26</v>
+        <v>25.5</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -4504,12 +4179,8 @@
       <c r="J7" s="18">
         <v>0</v>
       </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
@@ -4560,12 +4231,8 @@
       <c r="J8" s="18">
         <v>0</v>
       </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
@@ -4616,12 +4283,8 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -4652,7 +4315,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="18">
         <v>0</v>
@@ -4672,12 +4335,8 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <v>0</v>
-      </c>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
@@ -4714,26 +4373,22 @@
         <v>0</v>
       </c>
       <c r="F11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="18">
         <v>0</v>
       </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
@@ -4761,35 +4416,31 @@
         <v>0</v>
       </c>
       <c r="C12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="18">
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" s="18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I12" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -4823,29 +4474,25 @@
         <v>0</v>
       </c>
       <c r="E13" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G13" s="18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H13" s="18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -4882,26 +4529,22 @@
         <v>0</v>
       </c>
       <c r="F14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="18">
         <v>0</v>
       </c>
       <c r="I14" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J14" s="18">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
@@ -4944,20 +4587,16 @@
         <v>0</v>
       </c>
       <c r="H15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -4981,39 +4620,17 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>1</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0</v>
-      </c>
-      <c r="K16" s="18">
-        <v>0</v>
-      </c>
-      <c r="L16" s="18">
-        <v>0</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -5037,39 +4654,17 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0</v>
-      </c>
-      <c r="D17" s="18">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18">
-        <v>0</v>
-      </c>
-      <c r="F17" s="18">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18">
-        <v>5</v>
-      </c>
-      <c r="H17" s="18">
-        <v>2</v>
-      </c>
-      <c r="I17" s="18">
-        <v>1</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -5093,39 +4688,17 @@
       <c r="AG17" s="18"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0</v>
-      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -5149,39 +4722,17 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <v>1</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-      <c r="G19" s="18">
-        <v>2</v>
-      </c>
-      <c r="H19" s="18">
-        <v>6</v>
-      </c>
-      <c r="I19" s="18">
-        <v>1</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0</v>
-      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -5205,39 +4756,17 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
-        <v>0</v>
-      </c>
-      <c r="F20" s="18">
-        <v>1</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>2</v>
-      </c>
-      <c r="I20" s="18">
-        <v>2</v>
-      </c>
-      <c r="J20" s="18">
-        <v>1</v>
-      </c>
-      <c r="K20" s="18">
-        <v>0</v>
-      </c>
-      <c r="L20" s="18">
-        <v>0</v>
-      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -5261,39 +4790,17 @@
       <c r="AG20" s="18"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="18">
-        <v>4</v>
-      </c>
-      <c r="H21" s="18">
-        <v>6</v>
-      </c>
-      <c r="I21" s="18">
-        <v>2</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0</v>
-      </c>
-      <c r="K21" s="18">
-        <v>0</v>
-      </c>
-      <c r="L21" s="18">
-        <v>0</v>
-      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -5317,39 +4824,17 @@
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B22" s="18">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <v>4</v>
-      </c>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <v>2</v>
-      </c>
-      <c r="I22" s="18">
-        <v>1</v>
-      </c>
-      <c r="J22" s="18">
-        <v>1</v>
-      </c>
-      <c r="K22" s="18">
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
-        <v>0</v>
-      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -5373,39 +4858,17 @@
       <c r="AG22" s="18"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0</v>
-      </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>2</v>
-      </c>
-      <c r="H23" s="18">
-        <v>3</v>
-      </c>
-      <c r="I23" s="18">
-        <v>3</v>
-      </c>
-      <c r="J23" s="18">
-        <v>2</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
-        <v>0</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
@@ -5429,39 +4892,17 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B24" s="18">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>1</v>
-      </c>
-      <c r="H24" s="18">
-        <v>1</v>
-      </c>
-      <c r="I24" s="18">
-        <v>1</v>
-      </c>
-      <c r="J24" s="18">
-        <v>7</v>
-      </c>
-      <c r="K24" s="18">
-        <v>0</v>
-      </c>
-      <c r="L24" s="18">
-        <v>0</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
@@ -5485,39 +4926,17 @@
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>1</v>
-      </c>
-      <c r="G25" s="18">
-        <v>1</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <v>2</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <v>0</v>
-      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
@@ -5541,39 +4960,17 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B26" s="18">
-        <v>0</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0</v>
-      </c>
-      <c r="D26" s="18">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="18">
-        <v>2</v>
-      </c>
-      <c r="J26" s="18">
-        <v>1</v>
-      </c>
-      <c r="K26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <v>0</v>
-      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -5597,39 +4994,17 @@
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B27" s="18">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0</v>
-      </c>
-      <c r="D27" s="18">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <v>0</v>
-      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -5653,39 +5028,17 @@
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <v>0</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18">
-        <v>0</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
-        <v>1</v>
-      </c>
-      <c r="L28" s="18">
-        <v>0</v>
-      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
@@ -6066,8 +5419,8 @@
     <col min="1" max="1" width="17.21875" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.77734375" style="20" customWidth="1"/>
     <col min="6" max="34" width="7.77734375" style="20" customWidth="1"/>
-    <col min="35" max="36" width="8.88671875" style="7" customWidth="1"/>
-    <col min="37" max="16384" width="8.88671875" style="7"/>
+    <col min="35" max="39" width="8.88671875" style="7" customWidth="1"/>
+    <col min="40" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -6192,15 +5545,15 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="9.77734375" style="20" customWidth="1"/>
     <col min="5" max="33" width="7.77734375" style="20" customWidth="1"/>
-    <col min="34" max="35" width="8.88671875" style="7" customWidth="1"/>
-    <col min="36" max="16384" width="8.88671875" style="7"/>
+    <col min="34" max="38" width="8.88671875" style="7" customWidth="1"/>
+    <col min="39" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6238,7 +5591,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D3" s="6">
         <v>0.89854000000000001</v>
@@ -6249,10 +5602,10 @@
         <v>66</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D4" s="6">
         <v>0.65558000000000005</v>
@@ -6263,10 +5616,10 @@
         <v>70</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D5" s="6">
         <v>0.19886000000000001</v>
@@ -6277,10 +5630,10 @@
         <v>69</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D6" s="6">
         <v>5.645E-2</v>
@@ -6301,7 +5654,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6432,7 +5785,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -6479,7 +5832,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="18">
         <v>1</v>
@@ -6491,7 +5844,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="18">
         <v>0</v>
@@ -6508,12 +5861,8 @@
       <c r="J7" s="18">
         <v>0</v>
       </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
@@ -6539,19 +5888,19 @@
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="18">
         <v>0</v>
@@ -6565,12 +5914,8 @@
       <c r="J8" s="18">
         <v>0</v>
       </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
@@ -6595,22 +5940,22 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="18">
         <v>0</v>
       </c>
       <c r="D9" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="18">
         <v>0</v>
@@ -6621,12 +5966,8 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -6654,20 +5995,20 @@
         <v>0</v>
       </c>
       <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>13</v>
+      </c>
+      <c r="E10" s="18">
+        <v>11</v>
+      </c>
+      <c r="F10" s="18">
+        <v>7</v>
+      </c>
+      <c r="G10" s="18">
         <v>1</v>
       </c>
-      <c r="D10" s="18">
-        <v>1</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
       <c r="H10" s="18">
         <v>0</v>
       </c>
@@ -6677,12 +6018,8 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <v>0</v>
-      </c>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
@@ -6710,22 +6047,22 @@
         <v>0</v>
       </c>
       <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18">
         <v>2</v>
       </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
       <c r="E11" s="18">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F11" s="18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="18">
         <v>0</v>
@@ -6733,12 +6070,8 @@
       <c r="J11" s="18">
         <v>0</v>
       </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
@@ -6766,13 +6099,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="18">
+        <v>0</v>
+      </c>
+      <c r="D12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="E12" s="18">
         <v>1</v>
-      </c>
-      <c r="E12" s="18">
-        <v>0</v>
       </c>
       <c r="F12" s="18">
         <v>1</v>
@@ -6789,12 +6122,8 @@
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -6819,7 +6148,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="18">
         <v>0</v>
@@ -6828,13 +6157,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" s="18">
         <v>0</v>
@@ -6845,12 +6174,8 @@
       <c r="J13" s="18">
         <v>0</v>
       </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -6878,22 +6203,22 @@
         <v>0</v>
       </c>
       <c r="C14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="18">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E14" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="18">
         <v>0</v>
@@ -6901,12 +6226,8 @@
       <c r="J14" s="18">
         <v>0</v>
       </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
@@ -6940,13 +6261,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="18">
         <v>0</v>
@@ -6957,12 +6278,8 @@
       <c r="J15" s="18">
         <v>0</v>
       </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -6986,39 +6303,17 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>2</v>
-      </c>
-      <c r="E16" s="18">
-        <v>2</v>
-      </c>
-      <c r="F16" s="18">
-        <v>4</v>
-      </c>
-      <c r="G16" s="18">
-        <v>2</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0</v>
-      </c>
-      <c r="K16" s="18">
-        <v>0</v>
-      </c>
-      <c r="L16" s="18">
-        <v>0</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -7042,39 +6337,17 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0</v>
-      </c>
-      <c r="D17" s="18">
-        <v>1</v>
-      </c>
-      <c r="E17" s="18">
-        <v>4</v>
-      </c>
-      <c r="F17" s="18">
-        <v>8</v>
-      </c>
-      <c r="G17" s="18">
-        <v>1</v>
-      </c>
-      <c r="H17" s="18">
-        <v>0</v>
-      </c>
-      <c r="I17" s="18">
-        <v>0</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -7098,39 +6371,17 @@
       <c r="AG17" s="18"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>2</v>
-      </c>
-      <c r="F18" s="18">
-        <v>4</v>
-      </c>
-      <c r="G18" s="18">
-        <v>4</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0</v>
-      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -7154,39 +6405,17 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <v>1</v>
-      </c>
-      <c r="E19" s="18">
-        <v>1</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0</v>
-      </c>
-      <c r="I19" s="18">
-        <v>0</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0</v>
-      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -7210,39 +6439,17 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0</v>
-      </c>
-      <c r="I20" s="18">
-        <v>0</v>
-      </c>
-      <c r="J20" s="18">
-        <v>0</v>
-      </c>
-      <c r="K20" s="18">
-        <v>0</v>
-      </c>
-      <c r="L20" s="18">
-        <v>0</v>
-      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -7266,39 +6473,17 @@
       <c r="AG20" s="18"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0</v>
-      </c>
-      <c r="I21" s="18">
-        <v>0</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0</v>
-      </c>
-      <c r="K21" s="18">
-        <v>0</v>
-      </c>
-      <c r="L21" s="18">
-        <v>0</v>
-      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -7322,39 +6507,17 @@
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B22" s="18">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <v>0</v>
-      </c>
-      <c r="G22" s="18">
-        <v>1</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0</v>
-      </c>
-      <c r="I22" s="18">
-        <v>0</v>
-      </c>
-      <c r="J22" s="18">
-        <v>0</v>
-      </c>
-      <c r="K22" s="18">
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
-        <v>0</v>
-      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -7378,39 +6541,17 @@
       <c r="AG22" s="18"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0</v>
-      </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
-        <v>0</v>
-      </c>
-      <c r="J23" s="18">
-        <v>0</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
-        <v>0</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
@@ -7434,39 +6575,17 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B24" s="18">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <v>0</v>
-      </c>
-      <c r="I24" s="18">
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
-        <v>0</v>
-      </c>
-      <c r="K24" s="18">
-        <v>0</v>
-      </c>
-      <c r="L24" s="18">
-        <v>0</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
@@ -7490,39 +6609,17 @@
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <v>0</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <v>0</v>
-      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
@@ -7546,39 +6643,17 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B26" s="18">
-        <v>0</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0</v>
-      </c>
-      <c r="D26" s="18">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="18">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
-        <v>0</v>
-      </c>
-      <c r="K26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <v>0</v>
-      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -7602,39 +6677,17 @@
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B27" s="18">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0</v>
-      </c>
-      <c r="D27" s="18">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <v>0</v>
-      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -7658,39 +6711,17 @@
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <v>0</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18">
-        <v>0</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
-        <v>0</v>
-      </c>
-      <c r="L28" s="18">
-        <v>0</v>
-      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
@@ -8065,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8197,7 +7228,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -8244,7 +7275,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="18">
         <v>0</v>
@@ -8273,12 +7304,8 @@
       <c r="J7" s="18">
         <v>0</v>
       </c>
-      <c r="K7" s="18">
-        <v>0</v>
-      </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
@@ -8330,12 +7357,8 @@
       <c r="J8" s="18">
         <v>0</v>
       </c>
-      <c r="K8" s="18">
-        <v>0</v>
-      </c>
-      <c r="L8" s="18">
-        <v>0</v>
-      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
@@ -8386,12 +7409,8 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="18">
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
-        <v>0</v>
-      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -8422,7 +7441,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="18">
         <v>0</v>
@@ -8442,12 +7461,8 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
-        <v>0</v>
-      </c>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
@@ -8484,26 +7499,22 @@
         <v>0</v>
       </c>
       <c r="F11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="18">
         <v>0</v>
       </c>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="18">
-        <v>0</v>
-      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
@@ -8531,35 +7542,31 @@
         <v>0</v>
       </c>
       <c r="C12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="18">
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" s="18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I12" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="18">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <v>0</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -8593,29 +7600,25 @@
         <v>0</v>
       </c>
       <c r="E13" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G13" s="18">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H13" s="18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="18">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0</v>
-      </c>
-      <c r="L13" s="18">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -8652,26 +7655,22 @@
         <v>0</v>
       </c>
       <c r="F14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="18">
         <v>0</v>
       </c>
       <c r="I14" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J14" s="18">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
@@ -8714,20 +7713,16 @@
         <v>0</v>
       </c>
       <c r="H15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -8751,39 +7746,17 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>1</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <v>0</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <v>0</v>
-      </c>
-      <c r="K16" s="18">
-        <v>0</v>
-      </c>
-      <c r="L16" s="18">
-        <v>0</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -8807,39 +7780,17 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0</v>
-      </c>
-      <c r="D17" s="18">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18">
-        <v>0</v>
-      </c>
-      <c r="F17" s="18">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18">
-        <v>5</v>
-      </c>
-      <c r="H17" s="18">
-        <v>2</v>
-      </c>
-      <c r="I17" s="18">
-        <v>1</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -8863,39 +7814,17 @@
       <c r="AG17" s="18"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0</v>
-      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -8919,39 +7848,17 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <v>1</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-      <c r="G19" s="18">
-        <v>2</v>
-      </c>
-      <c r="H19" s="18">
-        <v>6</v>
-      </c>
-      <c r="I19" s="18">
-        <v>1</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0</v>
-      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -8975,39 +7882,17 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
-        <v>0</v>
-      </c>
-      <c r="F20" s="18">
-        <v>1</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
-        <v>2</v>
-      </c>
-      <c r="I20" s="18">
-        <v>2</v>
-      </c>
-      <c r="J20" s="18">
-        <v>1</v>
-      </c>
-      <c r="K20" s="18">
-        <v>0</v>
-      </c>
-      <c r="L20" s="18">
-        <v>0</v>
-      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -9031,39 +7916,17 @@
       <c r="AG20" s="18"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="18">
-        <v>4</v>
-      </c>
-      <c r="H21" s="18">
-        <v>6</v>
-      </c>
-      <c r="I21" s="18">
-        <v>2</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0</v>
-      </c>
-      <c r="K21" s="18">
-        <v>0</v>
-      </c>
-      <c r="L21" s="18">
-        <v>0</v>
-      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -9087,39 +7950,17 @@
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B22" s="18">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <v>4</v>
-      </c>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <v>2</v>
-      </c>
-      <c r="I22" s="18">
-        <v>1</v>
-      </c>
-      <c r="J22" s="18">
-        <v>1</v>
-      </c>
-      <c r="K22" s="18">
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
-        <v>0</v>
-      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -9143,39 +7984,17 @@
       <c r="AG22" s="18"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18">
-        <v>0</v>
-      </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>2</v>
-      </c>
-      <c r="H23" s="18">
-        <v>3</v>
-      </c>
-      <c r="I23" s="18">
-        <v>3</v>
-      </c>
-      <c r="J23" s="18">
-        <v>2</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
-        <v>0</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
@@ -9199,39 +8018,17 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B24" s="18">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>1</v>
-      </c>
-      <c r="H24" s="18">
-        <v>1</v>
-      </c>
-      <c r="I24" s="18">
-        <v>1</v>
-      </c>
-      <c r="J24" s="18">
-        <v>7</v>
-      </c>
-      <c r="K24" s="18">
-        <v>0</v>
-      </c>
-      <c r="L24" s="18">
-        <v>0</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
@@ -9255,39 +8052,17 @@
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>1</v>
-      </c>
-      <c r="G25" s="18">
-        <v>1</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <v>2</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <v>0</v>
-      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
@@ -9311,39 +8086,17 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B26" s="18">
-        <v>0</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0</v>
-      </c>
-      <c r="D26" s="18">
-        <v>0</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="18">
-        <v>2</v>
-      </c>
-      <c r="J26" s="18">
-        <v>1</v>
-      </c>
-      <c r="K26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <v>0</v>
-      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -9367,39 +8120,17 @@
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B27" s="18">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18">
-        <v>0</v>
-      </c>
-      <c r="D27" s="18">
-        <v>0</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <v>0</v>
-      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -9423,39 +8154,17 @@
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
-        <v>0</v>
-      </c>
-      <c r="C28" s="18">
-        <v>0</v>
-      </c>
-      <c r="D28" s="18">
-        <v>0</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18">
-        <v>0</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
-        <v>1</v>
-      </c>
-      <c r="L28" s="18">
-        <v>0</v>
-      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
@@ -9824,13 +8533,13 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="113.88671875" style="7" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="7"/>
+    <col min="2" max="6" width="8.88671875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="304.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>